<commit_message>
Changed method names and updated load test data method
</commit_message>
<xml_diff>
--- a/TestCoverage.xlsx
+++ b/TestCoverage.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cigniti\POCs\Prospects\Temenos\TemenosAutomation\Temenos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\POC\Temenos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A11B3A2-0AAC-4003-ADFF-CBD9AFBF5AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8EBF8A-40CD-4232-AB1D-FEA7253DE2B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{689EFBE4-52D1-4E17-8534-EA0109110271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{689EFBE4-52D1-4E17-8534-EA0109110271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -59,18 +60,6 @@
     <t>Sr.No</t>
   </si>
   <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Disburse</t>
-  </si>
-  <si>
-    <t>ManualReject</t>
-  </si>
-  <si>
-    <t>Manual Reject</t>
-  </si>
-  <si>
     <t>AutomatedTest\FunctionalTest\ManualReject\XYZ.cs</t>
   </si>
   <si>
@@ -84,6 +73,30 @@
   </si>
   <si>
     <t>þ</t>
+  </si>
+  <si>
+    <t>Decision Process</t>
+  </si>
+  <si>
+    <t>TestManualReject</t>
+  </si>
+  <si>
+    <t>TestDisbursement</t>
+  </si>
+  <si>
+    <t>TestAutoDecisionProcess</t>
+  </si>
+  <si>
+    <t>Test validates approval/rejection/review for loan</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Test validates addition and removal of applicants from system</t>
+  </si>
+  <si>
+    <t>TestAddVerifyRemoveApplicant</t>
   </si>
 </sst>
 </file>
@@ -131,13 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -146,6 +156,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -462,17 +478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE5B266-71AF-432D-B646-8A4BF51DD7CE}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
@@ -501,14 +517,14 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G2" s="1" t="s">
@@ -522,37 +538,61 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>17</v>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="G1:L1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>